<commit_message>
Updates to documentation for CRAN submission
</commit_message>
<xml_diff>
--- a/inst/extdata/exampleData.xlsx
+++ b/inst/extdata/exampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityhealthnetwork-my.sharepoint.com/personal/lisa_avery_uhnresearch_ca/Documents/exceldata/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DD8AC65-428D-43BE-B191-5C70CE34D7C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{4DD8AC65-428D-43BE-B191-5C70CE34D7C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{27163E6E-26FD-41DD-81CF-B6CDE5E79C9C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{91EC5246-433D-4887-A7C1-CEFB5E7FF033}"/>
   </bookViews>
@@ -16,9 +16,6 @@
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
     <sheet name="DataEntry" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="41">
   <si>
     <t>VariableName</t>
   </si>
@@ -144,6 +141,24 @@
   <si>
     <t/>
   </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
 </sst>
 </file>
 
@@ -202,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -258,11 +273,124 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -445,97 +573,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -549,60 +586,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Example-Survey"/>
-      <sheetName val="Example-Survival"/>
-      <sheetName val="Check_codes_"/>
-      <sheetName val="DataEntry_codes_"/>
-      <sheetName val="DataEntry"/>
-      <sheetName val="DataDictionary"/>
-      <sheetName val="Instructions"/>
-      <sheetName val="FAQ"/>
-      <sheetName val="LongForm"/>
-      <sheetName val="WideForm"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="CreateDataEntrySheet"/>
-      <definedName name="FormatDataEntry"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08BF9306-99E6-45F9-907E-EBE5235E1A89}" name="DataEntry_tbl" displayName="DataEntry_tbl" ref="A1:I109" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08BF9306-99E6-45F9-907E-EBE5235E1A89}" name="DataEntry_tbl" displayName="DataEntry_tbl" ref="A1:I109" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:I109" xr:uid="{8EF6DEFC-8F61-4520-B1EE-F96B7C7D3FAA}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{8F352FA5-33A7-4AC9-8228-5FF1687804BD}" name="ID" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{4EDB1C16-768E-4CCE-B4AD-8C92839B92DF}" name="Age" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{C949A334-D691-45C2-93D4-AB99E51BB35F}" name="Gender" dataDxfId="32">
-      <calculatedColumnFormula>IF(B1=1,"m","f")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{D1EB4EB8-DDD7-4960-B146-C2A5683207C2}" name="T_Stage" dataDxfId="31">
-      <calculatedColumnFormula>CONCATENATE("T",RANDBETWEEN(0,4))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{81449BB0-4C7C-4E00-B243-48624C86186E}" name="DxDate" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{FC0644FC-9E00-4E26-9F60-179F8ACE6966}" name="ECOG" dataDxfId="29">
-      <calculatedColumnFormula>RANDBETWEEN(0,5)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{F978A1EC-4A16-4D46-A185-608C1A2238D7}" name="Date_Death" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{BB2F31E0-53AA-4AC0-B10C-06EA9A5F924D}" name="Date_LFU" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{CE1EF736-BA3E-428C-9596-950E760F7B8B}" name="T0_Stg" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{8F352FA5-33A7-4AC9-8228-5FF1687804BD}" name="ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4EDB1C16-768E-4CCE-B4AD-8C92839B92DF}" name="Age" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{C949A334-D691-45C2-93D4-AB99E51BB35F}" name="Gender" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D1EB4EB8-DDD7-4960-B146-C2A5683207C2}" name="T_Stage" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{81449BB0-4C7C-4E00-B243-48624C86186E}" name="DxDate" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{FC0644FC-9E00-4E26-9F60-179F8ACE6966}" name="ECOG" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F978A1EC-4A16-4D46-A185-608C1A2238D7}" name="Date_Death" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{BB2F31E0-53AA-4AC0-B10C-06EA9A5F924D}" name="Date_LFU" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{CE1EF736-BA3E-428C-9596-950E760F7B8B}" name="T0_Stg" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1178,10 +1174,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160FE7A9-CF05-42CC-8F4C-B11B062F6F73}">
   <sheetPr codeName="Sheet26"/>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,9 +1190,10 @@
     <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1225,27 +1222,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>77</v>
       </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C65" si="0">IF(B1=1,"m","f")</f>
-        <v>f</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D65" ca="1" si="1">CONCATENATE("T",RANDBETWEEN(0,4))</f>
-        <v>T0</v>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="12">
         <v>43621</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F65" ca="1" si="2">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="12">
         <v>44414</v>
@@ -1254,27 +1248,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>58</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
       </c>
       <c r="E3" s="12">
         <v>43734</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="12">
         <v>43988</v>
@@ -1283,27 +1274,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>66</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" s="12">
         <v>43665</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>34</v>
@@ -1312,27 +1300,24 @@
         <v>44032</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>72</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
       </c>
       <c r="E5" s="12">
-        <v>43562</v>
+        <v>43816</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>34</v>
@@ -1341,27 +1326,24 @@
         <v>44381</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>52</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
       </c>
       <c r="E6" s="12">
         <v>43623</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="12">
         <v>44169</v>
@@ -1369,28 +1351,26 @@
       <c r="H6" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>72</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
       </c>
       <c r="E7" s="12">
         <v>44237</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="12">
         <v>44479</v>
@@ -1399,27 +1379,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>67</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="12">
         <v>43645</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="12">
         <v>44030</v>
@@ -1428,27 +1405,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>43</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
       <c r="E9" s="12">
         <v>44455</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G9" s="12">
         <v>44470</v>
@@ -1457,27 +1431,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>42</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="12">
         <v>43816</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>34</v>
@@ -1486,27 +1457,24 @@
         <v>44561</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>47</v>
       </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="12">
         <v>43655</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>34</v>
@@ -1515,27 +1483,24 @@
         <v>43824</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>72</v>
       </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="12">
         <v>44211</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="12">
         <v>44240</v>
@@ -1544,26 +1509,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>59</v>
       </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
       </c>
       <c r="E13" s="12">
         <v>44315</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G13" s="12">
@@ -1573,27 +1535,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>65</v>
       </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="12">
         <v>44169</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G14" s="12">
         <v>44334</v>
@@ -1602,27 +1561,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>74</v>
       </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="12">
         <v>43674</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>34</v>
@@ -1631,27 +1587,24 @@
         <v>44357</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>74</v>
       </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
       </c>
       <c r="E16" s="12">
         <v>44074</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G16" s="12">
         <v>44100</v>
@@ -1667,20 +1620,17 @@
       <c r="B17">
         <v>63</v>
       </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
       </c>
       <c r="E17" s="12">
         <v>43923</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G17" s="12">
         <v>44123</v>
@@ -1696,20 +1646,17 @@
       <c r="B18">
         <v>55</v>
       </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="12">
         <v>43882</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>34</v>
@@ -1725,20 +1672,17 @@
       <c r="B19">
         <v>83</v>
       </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
       </c>
       <c r="E19" s="12">
         <v>43793</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>34</v>
@@ -1754,19 +1698,16 @@
       <c r="B20">
         <v>65</v>
       </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
       </c>
       <c r="E20" s="12">
         <v>43701</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G20" s="12">
@@ -1783,20 +1724,17 @@
       <c r="B21">
         <v>74</v>
       </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
       </c>
       <c r="E21" s="12">
         <v>43983</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="12">
         <v>44173</v>
@@ -1812,20 +1750,17 @@
       <c r="B22">
         <v>84</v>
       </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
       </c>
       <c r="E22" s="12">
         <v>43640</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="12">
         <v>44442</v>
@@ -1841,20 +1776,17 @@
       <c r="B23">
         <v>41</v>
       </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
       </c>
       <c r="E23" s="12">
         <v>44158</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G23" s="12">
         <v>44307</v>
@@ -1870,20 +1802,17 @@
       <c r="B24">
         <v>41</v>
       </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
       </c>
       <c r="E24" s="12">
         <v>44445</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>34</v>
@@ -1899,20 +1828,17 @@
       <c r="B25">
         <v>46</v>
       </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
       </c>
       <c r="E25" s="12">
         <v>43477</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>34</v>
@@ -1928,20 +1854,17 @@
       <c r="B26">
         <v>70</v>
       </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
       </c>
       <c r="E26" s="12">
         <v>43870</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G26" s="12">
         <v>44099</v>
@@ -1957,20 +1880,17 @@
       <c r="B27">
         <v>70</v>
       </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
       </c>
       <c r="E27" s="12">
         <v>43795</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>34</v>
@@ -1986,20 +1906,17 @@
       <c r="B28">
         <v>40</v>
       </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
       </c>
       <c r="E28" s="12">
         <v>43480</v>
       </c>
       <c r="F28">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="12">
         <v>43790</v>
@@ -2015,20 +1932,17 @@
       <c r="B29">
         <v>84</v>
       </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
       </c>
       <c r="E29" s="12">
         <v>43988</v>
       </c>
       <c r="F29">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>34</v>
@@ -2044,20 +1958,17 @@
       <c r="B30">
         <v>56</v>
       </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
       </c>
       <c r="E30" s="12">
         <v>44376</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="12">
         <v>44383</v>
@@ -2073,20 +1984,17 @@
       <c r="B31">
         <v>71</v>
       </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
       </c>
       <c r="E31" s="12">
         <v>43753</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>34</v>
@@ -2102,20 +2010,17 @@
       <c r="B32">
         <v>83</v>
       </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
       </c>
       <c r="E32" s="12">
         <v>43652</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G32" s="12">
         <v>44104</v>
@@ -2131,20 +2036,17 @@
       <c r="B33">
         <v>73</v>
       </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
       </c>
       <c r="E33" s="12">
         <v>44475</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>34</v>
@@ -2160,19 +2062,16 @@
       <c r="B34">
         <v>50</v>
       </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
       </c>
       <c r="E34" s="12">
         <v>44365</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G34" s="12">
@@ -2189,20 +2088,17 @@
       <c r="B35">
         <v>54</v>
       </c>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
       </c>
       <c r="E35" s="12">
         <v>43630</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="12">
         <v>43669</v>
@@ -2218,20 +2114,17 @@
       <c r="B36">
         <v>64</v>
       </c>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
       </c>
       <c r="E36" s="12">
         <v>43775</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" s="12">
         <v>44043</v>
@@ -2247,20 +2140,17 @@
       <c r="B37">
         <v>83</v>
       </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
       </c>
       <c r="E37" s="12">
         <v>43468</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G37" s="12">
         <v>44060</v>
@@ -2276,20 +2166,17 @@
       <c r="B38">
         <v>56</v>
       </c>
-      <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
       </c>
       <c r="E38" s="12">
         <v>44001</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>34</v>
@@ -2305,20 +2192,17 @@
       <c r="B39">
         <v>70</v>
       </c>
-      <c r="C39" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
       </c>
       <c r="E39" s="12">
         <v>44148</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>34</v>
@@ -2334,20 +2218,17 @@
       <c r="B40">
         <v>77</v>
       </c>
-      <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>40</v>
       </c>
       <c r="E40" s="12">
         <v>43658</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" s="12">
         <v>43848</v>
@@ -2363,19 +2244,16 @@
       <c r="B41">
         <v>41</v>
       </c>
-      <c r="C41" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
       </c>
       <c r="E41" s="12">
         <v>43973</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G41" s="12" t="s">
@@ -2392,19 +2270,16 @@
       <c r="B42">
         <v>45</v>
       </c>
-      <c r="C42" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
       </c>
       <c r="E42" s="12">
         <v>44335</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G42" s="12">
@@ -2421,20 +2296,17 @@
       <c r="B43">
         <v>43</v>
       </c>
-      <c r="C43" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
       </c>
       <c r="E43" s="12">
         <v>43657</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>34</v>
@@ -2450,20 +2322,17 @@
       <c r="B44">
         <v>62</v>
       </c>
-      <c r="C44" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
       </c>
       <c r="E44" s="12">
         <v>43707</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>34</v>
@@ -2479,19 +2348,16 @@
       <c r="B45">
         <v>75</v>
       </c>
-      <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s">
+        <v>39</v>
       </c>
       <c r="E45" s="12">
         <v>44002</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G45" s="12" t="s">
@@ -2508,20 +2374,17 @@
       <c r="B46">
         <v>58</v>
       </c>
-      <c r="C46" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
+        <v>38</v>
       </c>
       <c r="E46" s="12">
         <v>44191</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" s="12">
         <v>44260</v>
@@ -2537,20 +2400,17 @@
       <c r="B47">
         <v>43</v>
       </c>
-      <c r="C47" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
       </c>
       <c r="E47" s="12">
         <v>44110</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>34</v>
@@ -2566,19 +2426,16 @@
       <c r="B48">
         <v>85</v>
       </c>
-      <c r="C48" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
       </c>
       <c r="E48" s="12">
         <v>43986</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G48" s="12">
@@ -2595,20 +2452,17 @@
       <c r="B49">
         <v>68</v>
       </c>
-      <c r="C49" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>40</v>
       </c>
       <c r="E49" s="12">
         <v>43845</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="12">
         <v>44117</v>
@@ -2624,19 +2478,16 @@
       <c r="B50">
         <v>81</v>
       </c>
-      <c r="C50" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
+        <v>38</v>
       </c>
       <c r="E50" s="12">
         <v>43551</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
       <c r="G50" s="12">
@@ -2653,20 +2504,17 @@
       <c r="B51">
         <v>46</v>
       </c>
-      <c r="C51" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" t="s">
+        <v>37</v>
       </c>
       <c r="E51" s="12">
         <v>44412</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>34</v>
@@ -2682,20 +2530,17 @@
       <c r="B52">
         <v>71</v>
       </c>
-      <c r="C52" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" t="s">
+        <v>40</v>
       </c>
       <c r="E52" s="12">
         <v>44354</v>
       </c>
       <c r="F52">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>34</v>
@@ -2711,19 +2556,16 @@
       <c r="B53">
         <v>70</v>
       </c>
-      <c r="C53" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" t="s">
+        <v>36</v>
       </c>
       <c r="E53" s="12">
         <v>43483</v>
       </c>
       <c r="F53">
-        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
       <c r="G53" s="12" t="s">
@@ -2740,20 +2582,17 @@
       <c r="B54">
         <v>65</v>
       </c>
-      <c r="C54" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" t="s">
+        <v>36</v>
       </c>
       <c r="E54" s="12">
         <v>43681</v>
       </c>
       <c r="F54">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G54" s="12">
         <v>44146</v>
@@ -2769,20 +2608,17 @@
       <c r="B55">
         <v>43</v>
       </c>
-      <c r="C55" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" t="s">
+        <v>39</v>
       </c>
       <c r="E55" s="12">
         <v>43692</v>
       </c>
       <c r="F55">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>34</v>
@@ -2798,20 +2634,17 @@
       <c r="B56">
         <v>56</v>
       </c>
-      <c r="C56" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T1</v>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" t="s">
+        <v>40</v>
       </c>
       <c r="E56" s="12">
         <v>44055</v>
       </c>
       <c r="F56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G56" s="12" t="s">
         <v>34</v>
@@ -2827,19 +2660,16 @@
       <c r="B57">
         <v>52</v>
       </c>
-      <c r="C57" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
       </c>
       <c r="E57" s="12">
         <v>44320</v>
       </c>
       <c r="F57">
-        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G57" s="12" t="s">
@@ -2856,20 +2686,17 @@
       <c r="B58">
         <v>56</v>
       </c>
-      <c r="C58" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" t="s">
+        <v>39</v>
       </c>
       <c r="E58" s="12">
         <v>44287</v>
       </c>
       <c r="F58">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G58" s="12">
         <v>44417</v>
@@ -2885,19 +2712,16 @@
       <c r="B59">
         <v>45</v>
       </c>
-      <c r="C59" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" t="s">
+        <v>40</v>
       </c>
       <c r="E59" s="12">
         <v>43699</v>
       </c>
       <c r="F59">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G59" s="12" t="s">
@@ -2914,20 +2738,17 @@
       <c r="B60">
         <v>48</v>
       </c>
-      <c r="C60" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" t="s">
+        <v>36</v>
       </c>
       <c r="E60" s="12">
         <v>44461</v>
       </c>
       <c r="F60">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G60" s="12">
         <v>44479</v>
@@ -2943,20 +2764,17 @@
       <c r="B61">
         <v>55</v>
       </c>
-      <c r="C61" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T0</v>
+      <c r="C61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" t="s">
+        <v>38</v>
       </c>
       <c r="E61" s="12">
         <v>43579</v>
       </c>
       <c r="F61">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G61" s="12">
         <v>44125</v>
@@ -2972,20 +2790,17 @@
       <c r="B62">
         <v>40</v>
       </c>
-      <c r="C62" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T2</v>
+      <c r="C62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" t="s">
+        <v>38</v>
       </c>
       <c r="E62" s="12">
         <v>43715</v>
       </c>
       <c r="F62">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G62" s="12">
         <v>44238</v>
@@ -3001,20 +2816,17 @@
       <c r="B63">
         <v>80</v>
       </c>
-      <c r="C63" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" t="s">
+        <v>36</v>
       </c>
       <c r="E63" s="12">
         <v>44006</v>
       </c>
       <c r="F63">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" s="12">
         <v>44314</v>
@@ -3030,20 +2842,17 @@
       <c r="B64">
         <v>44</v>
       </c>
-      <c r="C64" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T4</v>
+      <c r="C64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>36</v>
       </c>
       <c r="E64" s="12">
         <v>44048</v>
       </c>
       <c r="F64">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="12">
         <v>44369</v>
@@ -3059,20 +2868,17 @@
       <c r="B65">
         <v>68</v>
       </c>
-      <c r="C65" t="str">
-        <f t="shared" si="0"/>
-        <v>f</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>T3</v>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" t="s">
+        <v>37</v>
       </c>
       <c r="E65" s="12">
         <v>43967</v>
       </c>
       <c r="F65">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65" s="12" t="s">
         <v>34</v>
@@ -3088,20 +2894,17 @@
       <c r="B66">
         <v>51</v>
       </c>
-      <c r="C66" t="str">
-        <f t="shared" ref="C66:C109" si="3">IF(B65=1,"m","f")</f>
-        <v>f</v>
-      </c>
-      <c r="D66" t="str">
-        <f t="shared" ref="D66:D109" ca="1" si="4">CONCATENATE("T",RANDBETWEEN(0,4))</f>
-        <v>T0</v>
+      <c r="C66" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" t="s">
+        <v>36</v>
       </c>
       <c r="E66" s="12">
         <v>43696</v>
       </c>
       <c r="F66">
-        <f t="shared" ref="F66:F109" ca="1" si="5">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G66" s="12" t="s">
         <v>34</v>
@@ -3117,20 +2920,17 @@
       <c r="B67">
         <v>78</v>
       </c>
-      <c r="C67" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" t="s">
+        <v>38</v>
       </c>
       <c r="E67" s="12">
         <v>43963</v>
       </c>
       <c r="F67">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G67" s="12">
         <v>44367</v>
@@ -3146,20 +2946,17 @@
       <c r="B68">
         <v>60</v>
       </c>
-      <c r="C68" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D68" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" t="s">
+        <v>36</v>
       </c>
       <c r="E68" s="12">
         <v>44423</v>
       </c>
       <c r="F68">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>34</v>
@@ -3175,20 +2972,17 @@
       <c r="B69">
         <v>50</v>
       </c>
-      <c r="C69" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D69" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" t="s">
+        <v>38</v>
       </c>
       <c r="E69" s="12">
         <v>43871</v>
       </c>
       <c r="F69">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G69" s="12">
         <v>44160</v>
@@ -3204,19 +2998,16 @@
       <c r="B70">
         <v>51</v>
       </c>
-      <c r="C70" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D70" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" t="s">
+        <v>39</v>
       </c>
       <c r="E70" s="12">
         <v>43873</v>
       </c>
       <c r="F70">
-        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="G70" s="12" t="s">
@@ -3233,20 +3024,17 @@
       <c r="B71">
         <v>82</v>
       </c>
-      <c r="C71" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T0</v>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" t="s">
+        <v>38</v>
       </c>
       <c r="E71" s="12">
         <v>44356</v>
       </c>
       <c r="F71">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G71" s="12" t="s">
         <v>34</v>
@@ -3262,20 +3050,17 @@
       <c r="B72">
         <v>65</v>
       </c>
-      <c r="C72" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D72" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C72" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" t="s">
+        <v>39</v>
       </c>
       <c r="E72" s="12">
         <v>44241</v>
       </c>
       <c r="F72">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G72" s="12" t="s">
         <v>34</v>
@@ -3291,20 +3076,17 @@
       <c r="B73">
         <v>70</v>
       </c>
-      <c r="C73" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D73" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" t="s">
+        <v>36</v>
       </c>
       <c r="E73" s="12">
         <v>43571</v>
       </c>
       <c r="F73">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G73" s="12">
         <v>44259</v>
@@ -3320,20 +3102,17 @@
       <c r="B74">
         <v>65</v>
       </c>
-      <c r="C74" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D74" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T0</v>
+      <c r="C74" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" t="s">
+        <v>38</v>
       </c>
       <c r="E74" s="12">
         <v>43856</v>
       </c>
       <c r="F74">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G74" s="12" t="s">
         <v>34</v>
@@ -3349,20 +3128,17 @@
       <c r="B75">
         <v>81</v>
       </c>
-      <c r="C75" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D75" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" t="s">
+        <v>37</v>
       </c>
       <c r="E75" s="12">
         <v>43679</v>
       </c>
       <c r="F75">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="12">
         <v>44096</v>
@@ -3378,20 +3154,17 @@
       <c r="B76">
         <v>78</v>
       </c>
-      <c r="C76" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D76" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" t="s">
+        <v>40</v>
       </c>
       <c r="E76" s="12">
         <v>44270</v>
       </c>
       <c r="F76">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G76" s="12" t="s">
         <v>34</v>
@@ -3407,20 +3180,17 @@
       <c r="B77">
         <v>82</v>
       </c>
-      <c r="C77" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D77" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" t="s">
+        <v>39</v>
       </c>
       <c r="E77" s="12">
         <v>44390</v>
       </c>
       <c r="F77">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G77" s="12">
         <v>44437</v>
@@ -3436,20 +3206,17 @@
       <c r="B78">
         <v>54</v>
       </c>
-      <c r="C78" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D78" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C78" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" t="s">
+        <v>40</v>
       </c>
       <c r="E78" s="12">
         <v>43721</v>
       </c>
       <c r="F78">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>34</v>
@@ -3465,20 +3232,17 @@
       <c r="B79">
         <v>80</v>
       </c>
-      <c r="C79" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D79" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" t="s">
+        <v>37</v>
       </c>
       <c r="E79" s="12">
         <v>44316</v>
       </c>
       <c r="F79">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G79" s="12">
         <v>44369</v>
@@ -3494,19 +3258,16 @@
       <c r="B80">
         <v>46</v>
       </c>
-      <c r="C80" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D80" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C80" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" t="s">
+        <v>38</v>
       </c>
       <c r="E80" s="12">
         <v>44059</v>
       </c>
       <c r="F80">
-        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="G80" s="12">
@@ -3523,20 +3284,17 @@
       <c r="B81">
         <v>73</v>
       </c>
-      <c r="C81" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D81" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C81" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81" t="s">
+        <v>39</v>
       </c>
       <c r="E81" s="12">
         <v>43585</v>
       </c>
       <c r="F81">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>34</v>
@@ -3552,20 +3310,17 @@
       <c r="B82">
         <v>43</v>
       </c>
-      <c r="C82" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D82" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C82" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" t="s">
+        <v>40</v>
       </c>
       <c r="E82" s="12">
         <v>43490</v>
       </c>
       <c r="F82">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G82" s="12">
         <v>43608</v>
@@ -3581,20 +3336,17 @@
       <c r="B83">
         <v>80</v>
       </c>
-      <c r="C83" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C83" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" t="s">
+        <v>36</v>
       </c>
       <c r="E83" s="12">
         <v>43721</v>
       </c>
       <c r="F83">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G83" s="12">
         <v>44447</v>
@@ -3610,20 +3362,17 @@
       <c r="B84">
         <v>52</v>
       </c>
-      <c r="C84" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D84" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84" t="s">
+        <v>36</v>
       </c>
       <c r="E84" s="12">
         <v>43594</v>
       </c>
       <c r="F84">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>34</v>
@@ -3639,20 +3388,17 @@
       <c r="B85">
         <v>65</v>
       </c>
-      <c r="C85" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D85" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C85" t="s">
+        <v>35</v>
+      </c>
+      <c r="D85" t="s">
+        <v>40</v>
       </c>
       <c r="E85" s="12">
         <v>43780</v>
       </c>
       <c r="F85">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G85" s="12">
         <v>44212</v>
@@ -3668,19 +3414,16 @@
       <c r="B86">
         <v>45</v>
       </c>
-      <c r="C86" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D86" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T0</v>
+      <c r="C86" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" t="s">
+        <v>38</v>
       </c>
       <c r="E86" s="12">
         <v>43967</v>
       </c>
       <c r="F86">
-        <f t="shared" ca="1" si="5"/>
         <v>3</v>
       </c>
       <c r="G86" s="12" t="s">
@@ -3697,20 +3440,17 @@
       <c r="B87">
         <v>69</v>
       </c>
-      <c r="C87" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D87" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C87" t="s">
+        <v>35</v>
+      </c>
+      <c r="D87" t="s">
+        <v>40</v>
       </c>
       <c r="E87" s="12">
         <v>43780</v>
       </c>
       <c r="F87">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" s="12">
         <v>44405</v>
@@ -3726,20 +3466,17 @@
       <c r="B88">
         <v>84</v>
       </c>
-      <c r="C88" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D88" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88" t="s">
+        <v>40</v>
       </c>
       <c r="E88" s="12">
         <v>43698</v>
       </c>
       <c r="F88">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>34</v>
@@ -3755,20 +3492,17 @@
       <c r="B89">
         <v>46</v>
       </c>
-      <c r="C89" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D89" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C89" t="s">
+        <v>35</v>
+      </c>
+      <c r="D89" t="s">
+        <v>39</v>
       </c>
       <c r="E89" s="12">
         <v>44444</v>
       </c>
       <c r="F89">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>34</v>
@@ -3784,20 +3518,17 @@
       <c r="B90">
         <v>53</v>
       </c>
-      <c r="C90" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D90" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C90" t="s">
+        <v>35</v>
+      </c>
+      <c r="D90" t="s">
+        <v>40</v>
       </c>
       <c r="E90" s="12">
         <v>43508</v>
       </c>
       <c r="F90">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G90" s="12">
         <v>44139</v>
@@ -3813,20 +3544,17 @@
       <c r="B91">
         <v>50</v>
       </c>
-      <c r="C91" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D91" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C91" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" t="s">
+        <v>39</v>
       </c>
       <c r="E91" s="12">
         <v>44319</v>
       </c>
       <c r="F91">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>34</v>
@@ -3842,20 +3570,17 @@
       <c r="B92">
         <v>75</v>
       </c>
-      <c r="C92" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D92" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C92" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" t="s">
+        <v>38</v>
       </c>
       <c r="E92" s="12">
         <v>44258</v>
       </c>
       <c r="F92">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>34</v>
@@ -3871,20 +3596,17 @@
       <c r="B93">
         <v>80</v>
       </c>
-      <c r="C93" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D93" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T0</v>
+      <c r="C93" t="s">
+        <v>35</v>
+      </c>
+      <c r="D93" t="s">
+        <v>37</v>
       </c>
       <c r="E93" s="12">
         <v>44142</v>
       </c>
       <c r="F93">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>34</v>
@@ -3900,20 +3622,17 @@
       <c r="B94">
         <v>81</v>
       </c>
-      <c r="C94" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D94" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C94" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94" t="s">
+        <v>40</v>
       </c>
       <c r="E94" s="12">
         <v>44086</v>
       </c>
       <c r="F94">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>34</v>
@@ -3929,20 +3648,17 @@
       <c r="B95">
         <v>70</v>
       </c>
-      <c r="C95" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D95" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C95" t="s">
+        <v>35</v>
+      </c>
+      <c r="D95" t="s">
+        <v>37</v>
       </c>
       <c r="E95" s="12">
         <v>44300</v>
       </c>
       <c r="F95">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>34</v>
@@ -3958,19 +3674,16 @@
       <c r="B96">
         <v>54</v>
       </c>
-      <c r="C96" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D96" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C96" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96" t="s">
+        <v>36</v>
       </c>
       <c r="E96" s="12">
         <v>44283</v>
       </c>
       <c r="F96">
-        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="G96" s="12" t="s">
@@ -3987,20 +3700,17 @@
       <c r="B97">
         <v>47</v>
       </c>
-      <c r="C97" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D97" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C97" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" t="s">
+        <v>37</v>
       </c>
       <c r="E97" s="12">
         <v>43584</v>
       </c>
       <c r="F97">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G97" s="12" t="s">
         <v>34</v>
@@ -4016,20 +3726,17 @@
       <c r="B98">
         <v>43</v>
       </c>
-      <c r="C98" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D98" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C98" t="s">
+        <v>35</v>
+      </c>
+      <c r="D98" t="s">
+        <v>36</v>
       </c>
       <c r="E98" s="12">
         <v>43855</v>
       </c>
       <c r="F98">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>34</v>
@@ -4045,19 +3752,16 @@
       <c r="B99">
         <v>63</v>
       </c>
-      <c r="C99" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D99" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C99" t="s">
+        <v>35</v>
+      </c>
+      <c r="D99" t="s">
+        <v>36</v>
       </c>
       <c r="E99" s="12">
         <v>43662</v>
       </c>
       <c r="F99">
-        <f t="shared" ca="1" si="5"/>
         <v>3</v>
       </c>
       <c r="G99" s="12">
@@ -4074,20 +3778,17 @@
       <c r="B100">
         <v>52</v>
       </c>
-      <c r="C100" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D100" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T0</v>
+      <c r="C100" t="s">
+        <v>35</v>
+      </c>
+      <c r="D100" t="s">
+        <v>39</v>
       </c>
       <c r="E100" s="12">
         <v>43480</v>
       </c>
       <c r="F100">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G100" s="12" t="s">
         <v>34</v>
@@ -4103,20 +3804,17 @@
       <c r="B101">
         <v>74</v>
       </c>
-      <c r="C101" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D101" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C101" t="s">
+        <v>35</v>
+      </c>
+      <c r="D101" t="s">
+        <v>36</v>
       </c>
       <c r="E101" s="12">
         <v>44373</v>
       </c>
       <c r="F101">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G101" s="12">
         <v>44422</v>
@@ -4132,19 +3830,16 @@
       <c r="B102">
         <v>60</v>
       </c>
-      <c r="C102" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D102" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T2</v>
+      <c r="C102" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" t="s">
+        <v>36</v>
       </c>
       <c r="E102" s="12">
         <v>43539</v>
       </c>
       <c r="F102">
-        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="G102" s="12" t="s">
@@ -4161,20 +3856,17 @@
       <c r="B103">
         <v>84</v>
       </c>
-      <c r="C103" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D103" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C103" t="s">
+        <v>35</v>
+      </c>
+      <c r="D103" t="s">
+        <v>36</v>
       </c>
       <c r="E103" s="12">
         <v>43599</v>
       </c>
       <c r="F103">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="12">
         <v>44045</v>
@@ -4190,19 +3882,16 @@
       <c r="B104">
         <v>46</v>
       </c>
-      <c r="C104" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D104" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C104" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104" t="s">
+        <v>39</v>
       </c>
       <c r="E104" s="12">
         <v>43876</v>
       </c>
       <c r="F104">
-        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="G104" s="12" t="s">
@@ -4219,20 +3908,17 @@
       <c r="B105">
         <v>49</v>
       </c>
-      <c r="C105" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D105" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T4</v>
+      <c r="C105" t="s">
+        <v>35</v>
+      </c>
+      <c r="D105" t="s">
+        <v>40</v>
       </c>
       <c r="E105" s="12">
         <v>44425</v>
       </c>
       <c r="F105">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G105" s="12">
         <v>44439</v>
@@ -4248,20 +3934,17 @@
       <c r="B106">
         <v>72</v>
       </c>
-      <c r="C106" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D106" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C106" t="s">
+        <v>35</v>
+      </c>
+      <c r="D106" t="s">
+        <v>40</v>
       </c>
       <c r="E106" s="12">
         <v>44470</v>
       </c>
       <c r="F106">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G106" s="12">
         <v>44479</v>
@@ -4277,20 +3960,17 @@
       <c r="B107">
         <v>67</v>
       </c>
-      <c r="C107" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D107" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T1</v>
+      <c r="C107" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" t="s">
+        <v>38</v>
       </c>
       <c r="E107" s="12">
         <v>43545</v>
       </c>
       <c r="F107">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G107" s="12">
         <v>43749</v>
@@ -4306,20 +3986,17 @@
       <c r="B108">
         <v>79</v>
       </c>
-      <c r="C108" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D108" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C108" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108" t="s">
+        <v>38</v>
       </c>
       <c r="E108" s="12">
         <v>43718</v>
       </c>
       <c r="F108">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G108" s="12" t="s">
         <v>34</v>
@@ -4335,20 +4012,17 @@
       <c r="B109">
         <v>80</v>
       </c>
-      <c r="C109" t="str">
-        <f t="shared" si="3"/>
-        <v>f</v>
-      </c>
-      <c r="D109" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>T3</v>
+      <c r="C109" t="s">
+        <v>35</v>
+      </c>
+      <c r="D109" t="s">
+        <v>40</v>
       </c>
       <c r="E109" s="12">
         <v>43619</v>
       </c>
       <c r="F109">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G109" s="12">
         <v>44158</v>
@@ -4359,116 +4033,129 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="25" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="38" priority="18" stopIfTrue="1" operator="notBetween">
       <formula>40</formula>
       <formula>110</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B109">
-    <cfRule type="expression" dxfId="23" priority="12" stopIfTrue="1">
+  <conditionalFormatting sqref="B3:B16 B18:B109">
+    <cfRule type="expression" dxfId="37" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="13" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="36" priority="16" stopIfTrue="1" operator="notBetween">
       <formula>40</formula>
       <formula>110</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="17" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="34" priority="20" stopIfTrue="1" operator="notBetween">
       <formula>43466</formula>
       <formula>TODAY()</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="33" priority="21" stopIfTrue="1" operator="notBetween">
       <formula>43466</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E109">
-    <cfRule type="expression" dxfId="18" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="E3:E4 E6:E109">
+    <cfRule type="expression" dxfId="32" priority="12" stopIfTrue="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="31" priority="13" stopIfTrue="1" operator="notBetween">
       <formula>43466</formula>
       <formula>TODAY()</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="30" priority="14" stopIfTrue="1" operator="notBetween">
       <formula>43466</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(F2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="20" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="28" priority="23" stopIfTrue="1" operator="notBetween">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F109">
-    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="26" priority="11" stopIfTrue="1" operator="notBetween">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="24" stopIfTrue="1">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="22" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="notBetween">
       <formula>E2</formula>
       <formula>44561</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="23" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="23" priority="26" stopIfTrue="1" operator="notBetween">
       <formula>E2</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G109">
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="notBetween">
       <formula>E3</formula>
       <formula>44561</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="notBetween">
       <formula>E3</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="5" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="25" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="notBetween">
       <formula>E2</formula>
       <formula>44561</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="26" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="17" priority="29" stopIfTrue="1" operator="notBetween">
       <formula>E2</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H109">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(H3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="notBetween">
       <formula>E3</formula>
       <formula>44561</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" stopIfTrue="1" operator="notBetween">
+      <formula>E3</formula>
+      <formula>TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notBetween">
+      <formula>43466</formula>
+      <formula>TODAY()</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="notBetween">
-      <formula>E3</formula>
+      <formula>43466</formula>
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4496,7 +4183,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="Enter one of the allowed values:m,f" promptTitle="User Defined Codes" prompt="Enter one of the allowed values:m,f" sqref="C2:C109" xr:uid="{CC465ABC-8CCA-401D-8C21-707D54DB2CC3}">
       <formula1>"m,f"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numeric" error="Enter an numeric between 40 and 110" promptTitle="Numeric" prompt="Enter an numeric between 40 and 110" sqref="B2:B109" xr:uid="{E9805312-14C7-4CE5-BF51-BD4C212BDFDA}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numeric" error="Enter an numeric between 40 and 110" promptTitle="Numeric" prompt="Enter an numeric between 40 and 110" sqref="B2:B16 B18:B109" xr:uid="{E9805312-14C7-4CE5-BF51-BD4C212BDFDA}">
       <formula1>40</formula1>
       <formula2>110</formula2>
     </dataValidation>

</xml_diff>